<commit_message>
cleanup test files to try and inject unicode error
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-taxlots.xlsx
+++ b/seed/data_importer/tests/data/example-data-taxlots.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naddy/Source/LBL/seed/seed/data_importer/tests/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="2160" yWindow="8400" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Building data" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>521 Elm Street</t>
   </si>
@@ -39,15 +44,9 @@
     <t>address</t>
   </si>
   <si>
-    <t>jurisdiction_taxlot_identifier</t>
-  </si>
-  <si>
     <t>number_buildings</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>2655 Welstone Ave NE</t>
   </si>
   <si>
@@ -64,6 +63,9 @@
   </si>
   <si>
     <t>39929 Ranch 99 Road</t>
+  </si>
+  <si>
+    <t>jurisdiction_tax_lot_id</t>
   </si>
 </sst>
 </file>
@@ -683,12 +685,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -718,12 +720,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -927,184 +929,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1552813</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>11160509</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>13334485</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>23810533</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>24651456</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1552813</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="5" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>33366125</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5">
-        <v>1</v>
-      </c>
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5"/>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>11160509</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="5">
-        <v>2</v>
-      </c>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>33366148</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5"/>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>33366555</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5"/>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>33366125</v>
-      </c>
-      <c r="C5" s="2" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>55039309</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>33366148</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2">
-        <v>24651456</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5">
-        <v>13334485</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="3">
+      <c r="C10" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="B9" s="5">
-        <v>23810533</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5">
-        <v>55039309</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:D10">
+    <sortCondition ref="A2:A10"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>